<commit_message>
Added a Parameters class, Added a number generator function, started creating the function calculate an iteration of the MonteCarloProcess
</commit_message>
<xml_diff>
--- a/data/INPUT.xlsx
+++ b/data/INPUT.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joziv\Documents\AAA_projects\Calculo de inversion\Calculo-de-la-Rentabilidad\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A70BD9AE-4A21-4AA7-9079-F66B20F70E8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E2AB2F2-3753-44B4-AC55-F28518252856}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="caso abc imptos 10%" sheetId="8" r:id="rId1"/>
+    <sheet name="BaseCase" sheetId="8" r:id="rId1"/>
     <sheet name="Hoja blanco" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="26">
   <si>
     <t>Estudio de la rentabilidad: Planta ABC. SA</t>
   </si>
@@ -103,6 +103,15 @@
   </si>
   <si>
     <t>Estudio de la rentabilidad: Planta ABC. SA CASO BASE</t>
+  </si>
+  <si>
+    <t>Inversion</t>
+  </si>
+  <si>
+    <t>Costes operacion</t>
+  </si>
+  <si>
+    <t>Amortizacion</t>
   </si>
 </sst>
 </file>
@@ -942,8 +951,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1030,7 +1039,7 @@
     </row>
     <row r="4" spans="1:14" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="B4" s="14">
         <f>-0.2*$B$20</f>
@@ -1294,7 +1303,7 @@
     </row>
     <row r="10" spans="1:14" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A10" s="17" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="B10" s="18"/>
       <c r="C10" s="19"/>
@@ -1415,7 +1424,7 @@
     </row>
     <row r="13" spans="1:14" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A13" s="13" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="B13" s="29"/>
       <c r="C13" s="30"/>

</xml_diff>

<commit_message>
Created an Excel Handler class, and I also refactored the simulator, efficiency seems to have improved
</commit_message>
<xml_diff>
--- a/data/INPUT.xlsx
+++ b/data/INPUT.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joziv\Documents\AAA_projects\Calculo de inversion\Calculo-de-la-Rentabilidad\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A621BD75-4276-454E-A794-109D2BE097CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EBEE169-DBCA-487C-ADB6-9A96B2AB5AE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="19386" windowHeight="11466" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BaseCase" sheetId="8" r:id="rId1"/>
-    <sheet name="Hoja blanco" sheetId="4" r:id="rId2"/>
+    <sheet name="Multiplicadores" sheetId="9" r:id="rId2"/>
+    <sheet name="Hoja blanco" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="29">
   <si>
     <t>Estudio de la rentabilidad: Planta ABC. SA</t>
   </si>
@@ -112,6 +113,15 @@
   </si>
   <si>
     <t>Amortizacion</t>
+  </si>
+  <si>
+    <t>Ingresos</t>
+  </si>
+  <si>
+    <t>Costes Totales</t>
+  </si>
+  <si>
+    <t>Datos Proyecto multiplicados</t>
   </si>
 </sst>
 </file>
@@ -951,18 +961,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P10" sqref="P10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.52734375" defaultRowHeight="12.7" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="29.44140625" customWidth="1"/>
-    <col min="2" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.88671875" customWidth="1"/>
+    <col min="1" max="1" width="29.41015625" customWidth="1"/>
+    <col min="2" max="2" width="16.87890625" customWidth="1"/>
+    <col min="3" max="4" width="12.3515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.87890625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" ht="20" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="44" t="s">
         <v>0</v>
       </c>
@@ -980,8 +991,8 @@
       <c r="M1" s="46"/>
       <c r="N1" s="46"/>
     </row>
-    <row r="2" spans="1:14" ht="13.8" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:14" s="4" customFormat="1" ht="35.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" ht="13" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="3" spans="1:14" s="4" customFormat="1" ht="35.700000000000003" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A3" s="9" t="s">
         <v>16</v>
       </c>
@@ -1037,20 +1048,20 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" ht="17.7" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="13" t="s">
         <v>23</v>
       </c>
       <c r="B4" s="14">
-        <f>-0.2*$B$20</f>
+        <f>-0.2*$C$20</f>
         <v>-28000</v>
       </c>
       <c r="C4" s="15">
-        <f>-0.5*$B$20</f>
+        <f>-0.5*$C$20</f>
         <v>-70000</v>
       </c>
       <c r="D4" s="15">
-        <f>-0.3*$B$20</f>
+        <f>-0.3*$C$20</f>
         <v>-42000</v>
       </c>
       <c r="E4" s="15">
@@ -1084,7 +1095,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" ht="17.7" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="17" t="s">
         <v>12</v>
       </c>
@@ -1138,7 +1149,7 @@
         <v>7467.5519999999997</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" ht="17.7" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="17" t="s">
         <v>2</v>
       </c>
@@ -1160,31 +1171,31 @@
         <v>70200</v>
       </c>
       <c r="G6" s="19">
-        <f>($B$21*$B$25+$B$22*$B$26)</f>
+        <f>($B$21*$B$25+$B$22*$B$26)*Multiplicadores!B2</f>
         <v>78000</v>
       </c>
       <c r="H6" s="19">
-        <f>($B$21*$B$25+$B$22*$B$26)</f>
+        <f>($B$21*$B$25+$B$22*$B$26)*Multiplicadores!B2</f>
         <v>78000</v>
       </c>
       <c r="I6" s="19">
+        <f>1.05*($B$21*$B$25+$B$22*$B$26)*Multiplicadores!B2</f>
+        <v>81900</v>
+      </c>
+      <c r="J6" s="19">
+        <f>1.05*($B$21*$B$25+$B$22*$B$26)*Multiplicadores!B2</f>
+        <v>81900</v>
+      </c>
+      <c r="K6" s="19">
+        <f>1.05*($B$21*$B$25+$B$22*$B$26)*Multiplicadores!B2</f>
+        <v>81900</v>
+      </c>
+      <c r="L6" s="19">
+        <f>1.05*($B$21*$B$25+$B$22*$B$26)*Multiplicadores!B2</f>
+        <v>81900</v>
+      </c>
+      <c r="M6" s="19">
         <f t="shared" ref="I6:N6" si="2">1.05*($B$21*$B$25+$B$22*$B$26)</f>
-        <v>81900</v>
-      </c>
-      <c r="J6" s="19">
-        <f t="shared" si="2"/>
-        <v>81900</v>
-      </c>
-      <c r="K6" s="19">
-        <f t="shared" si="2"/>
-        <v>81900</v>
-      </c>
-      <c r="L6" s="19">
-        <f t="shared" si="2"/>
-        <v>81900</v>
-      </c>
-      <c r="M6" s="19">
-        <f t="shared" si="2"/>
         <v>81900</v>
       </c>
       <c r="N6" s="20">
@@ -1192,7 +1203,7 @@
         <v>81900</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" ht="17.7" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="17" t="s">
         <v>20</v>
       </c>
@@ -1206,39 +1217,39 @@
         <v>0</v>
       </c>
       <c r="E7" s="19">
-        <f t="shared" ref="E7:N7" si="3">SUM(E8:E10)</f>
+        <f>SUM(E8:E10)*Multiplicadores!$B$3</f>
         <v>18678.88</v>
       </c>
       <c r="F7" s="19">
-        <f t="shared" si="3"/>
+        <f>SUM(F8:F10)*Multiplicadores!$B$3</f>
         <v>22406.655999999999</v>
       </c>
       <c r="G7" s="19">
-        <f t="shared" si="3"/>
+        <f>SUM(G8:G10)*Multiplicadores!$B$3</f>
         <v>24891.84</v>
       </c>
       <c r="H7" s="19">
-        <f t="shared" si="3"/>
+        <f>SUM(H8:H10)*Multiplicadores!$B$3</f>
         <v>29870.207999999999</v>
       </c>
       <c r="I7" s="19">
-        <f t="shared" si="3"/>
+        <f>SUM(I8:I10)*Multiplicadores!$B$3</f>
         <v>29870.207999999999</v>
       </c>
       <c r="J7" s="19">
-        <f t="shared" si="3"/>
+        <f>SUM(J8:J10)*Multiplicadores!$B$3</f>
         <v>29870.207999999999</v>
       </c>
       <c r="K7" s="19">
-        <f t="shared" si="3"/>
+        <f>SUM(K8:K10)*Multiplicadores!$B$3</f>
         <v>29870.207999999999</v>
       </c>
       <c r="L7" s="19">
-        <f t="shared" si="3"/>
+        <f>SUM(L8:L10)*Multiplicadores!$B$3</f>
         <v>29870.207999999999</v>
       </c>
       <c r="M7" s="19">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="E7:N7" si="3">SUM(M8:M10)</f>
         <v>29870.207999999999</v>
       </c>
       <c r="N7" s="20">
@@ -1246,7 +1257,7 @@
         <v>29870.207999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" ht="17.7" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="17" t="s">
         <v>3</v>
       </c>
@@ -1297,7 +1308,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" ht="17.7" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="17" t="s">
         <v>4</v>
       </c>
@@ -1351,7 +1362,7 @@
         <v>29520</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" ht="17.7" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="17" t="s">
         <v>24</v>
       </c>
@@ -1405,7 +1416,7 @@
         <v>302.20799999999997</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" ht="18" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A11" s="21"/>
       <c r="B11" s="18">
         <v>0</v>
@@ -1447,7 +1458,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:14" s="1" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:14" s="1" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A12" s="25" t="s">
         <v>13</v>
       </c>
@@ -1464,7 +1475,7 @@
         <v>-42000</v>
       </c>
       <c r="E12" s="27">
-        <f t="shared" si="7"/>
+        <f>SUM(E4+E5+E6-E7)</f>
         <v>35151.399999999994</v>
       </c>
       <c r="F12" s="27">
@@ -1504,7 +1515,7 @@
         <v>59497.343999999997</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" ht="17.7" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="13" t="s">
         <v>25</v>
       </c>
@@ -1558,7 +1569,7 @@
         <v>14000</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" ht="17.7" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="17" t="s">
         <v>6</v>
       </c>
@@ -1612,7 +1623,7 @@
         <v>3802.9792000000002</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" ht="18" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A15" s="21"/>
       <c r="B15" s="18">
         <v>0</v>
@@ -1654,7 +1665,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:14" s="1" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:14" s="1" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A16" s="25" t="s">
         <v>14</v>
       </c>
@@ -1711,8 +1722,8 @@
         <v>55694.364799999996</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="13.8" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="18" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" ht="13" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="18" spans="1:10" ht="18" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A18" s="32" t="s">
         <v>21</v>
       </c>
@@ -1721,27 +1732,32 @@
         <v>0.22434040872513239</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A19" s="8" t="s">
         <v>7</v>
       </c>
       <c r="B19" s="8"/>
-      <c r="C19" s="1"/>
+      <c r="C19" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="D19" s="1"/>
       <c r="I19" s="5"/>
       <c r="J19" s="6"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A20" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B20" s="1">
         <v>140000</v>
       </c>
-      <c r="C20" s="1"/>
+      <c r="C20" s="1">
+        <f>B20*Multiplicadores!B1</f>
+        <v>140000</v>
+      </c>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A21" s="1" t="s">
         <v>9</v>
       </c>
@@ -1751,7 +1767,7 @@
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A22" s="1" t="s">
         <v>11</v>
       </c>
@@ -1761,7 +1777,7 @@
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A23" s="1" t="s">
         <v>10</v>
       </c>
@@ -1771,7 +1787,7 @@
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A24" s="8" t="s">
         <v>15</v>
       </c>
@@ -1779,7 +1795,7 @@
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A25" s="1" t="s">
         <v>9</v>
       </c>
@@ -1790,7 +1806,7 @@
       <c r="D25" s="1"/>
       <c r="F25" s="7"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A26" s="1" t="s">
         <v>11</v>
       </c>
@@ -1800,7 +1816,7 @@
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A27" s="1" t="s">
         <v>10</v>
       </c>
@@ -1810,7 +1826,7 @@
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A28" s="1" t="s">
         <v>18</v>
       </c>
@@ -1825,7 +1841,7 @@
         <v>247.5</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A29" s="1" t="s">
         <v>19</v>
       </c>
@@ -1852,6 +1868,48 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE702265-E10B-4C0E-9313-52523401792C}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.7" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="12.17578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:N29"/>
   <sheetViews>
@@ -1859,13 +1917,13 @@
       <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.52734375" defaultRowHeight="12.7" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="29.6640625" customWidth="1"/>
-    <col min="2" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.64453125" customWidth="1"/>
+    <col min="2" max="4" width="12.3515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" ht="20" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="44" t="s">
         <v>22</v>
       </c>
@@ -1883,8 +1941,8 @@
       <c r="M1" s="46"/>
       <c r="N1" s="46"/>
     </row>
-    <row r="2" spans="1:14" ht="13.8" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:14" s="4" customFormat="1" ht="35.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" ht="13" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="3" spans="1:14" s="4" customFormat="1" ht="35.700000000000003" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A3" s="37" t="s">
         <v>16</v>
       </c>
@@ -1940,7 +1998,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" ht="17.7" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="38" t="s">
         <v>1</v>
       </c>
@@ -1958,7 +2016,7 @@
       <c r="M4" s="15"/>
       <c r="N4" s="16"/>
     </row>
-    <row r="5" spans="1:14" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" ht="17.7" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="39" t="s">
         <v>12</v>
       </c>
@@ -1976,7 +2034,7 @@
       <c r="M5" s="19"/>
       <c r="N5" s="20"/>
     </row>
-    <row r="6" spans="1:14" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" ht="17.7" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="39" t="s">
         <v>2</v>
       </c>
@@ -1994,7 +2052,7 @@
       <c r="M6" s="19"/>
       <c r="N6" s="20"/>
     </row>
-    <row r="7" spans="1:14" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" ht="17.7" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="39" t="s">
         <v>20</v>
       </c>
@@ -2012,7 +2070,7 @@
       <c r="M7" s="19"/>
       <c r="N7" s="20"/>
     </row>
-    <row r="8" spans="1:14" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" ht="17.7" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="39" t="s">
         <v>3</v>
       </c>
@@ -2030,7 +2088,7 @@
       <c r="M8" s="19"/>
       <c r="N8" s="20"/>
     </row>
-    <row r="9" spans="1:14" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" ht="17.7" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="39" t="s">
         <v>4</v>
       </c>
@@ -2048,7 +2106,7 @@
       <c r="M9" s="19"/>
       <c r="N9" s="20"/>
     </row>
-    <row r="10" spans="1:14" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" ht="17.7" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="39" t="s">
         <v>17</v>
       </c>
@@ -2066,7 +2124,7 @@
       <c r="M10" s="19"/>
       <c r="N10" s="20"/>
     </row>
-    <row r="11" spans="1:14" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" ht="18" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A11" s="40"/>
       <c r="B11" s="22"/>
       <c r="C11" s="23"/>
@@ -2082,7 +2140,7 @@
       <c r="M11" s="23"/>
       <c r="N11" s="24"/>
     </row>
-    <row r="12" spans="1:14" s="1" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:14" s="1" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A12" s="41" t="s">
         <v>13</v>
       </c>
@@ -2100,7 +2158,7 @@
       <c r="M12" s="27"/>
       <c r="N12" s="28"/>
     </row>
-    <row r="13" spans="1:14" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" ht="17.7" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="38" t="s">
         <v>5</v>
       </c>
@@ -2118,7 +2176,7 @@
       <c r="M13" s="30"/>
       <c r="N13" s="31"/>
     </row>
-    <row r="14" spans="1:14" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" ht="17.7" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="39" t="s">
         <v>6</v>
       </c>
@@ -2136,7 +2194,7 @@
       <c r="M14" s="19"/>
       <c r="N14" s="19"/>
     </row>
-    <row r="15" spans="1:14" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" ht="18" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A15" s="40"/>
       <c r="B15" s="22"/>
       <c r="C15" s="23"/>
@@ -2152,7 +2210,7 @@
       <c r="M15" s="23"/>
       <c r="N15" s="24"/>
     </row>
-    <row r="16" spans="1:14" s="1" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:14" s="1" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A16" s="41" t="s">
         <v>14</v>
       </c>
@@ -2170,8 +2228,8 @@
       <c r="M16" s="27"/>
       <c r="N16" s="28"/>
     </row>
-    <row r="17" spans="1:6" ht="13.8" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="18" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" ht="13" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="18" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A18" s="42" t="s">
         <v>21</v>
       </c>
@@ -2180,40 +2238,40 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" ht="15.35" x14ac:dyDescent="0.5">
       <c r="A19" s="1"/>
       <c r="F19" s="3"/>
     </row>
-    <row r="20" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" ht="15.35" x14ac:dyDescent="0.5">
       <c r="A20" s="1"/>
       <c r="F20" s="3"/>
     </row>
-    <row r="21" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" ht="15.35" x14ac:dyDescent="0.5">
       <c r="A21" s="2"/>
       <c r="F21" s="3"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A22" s="2"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A23" s="2"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A24" s="1"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A25" s="2"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A26" s="2"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A27" s="2"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A28" s="2"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A29" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
We made it more efficient, by adding a multiplier on the excel file that already does everything and we don't have to manually multiply everything
</commit_message>
<xml_diff>
--- a/data/INPUT.xlsx
+++ b/data/INPUT.xlsx
@@ -8,14 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joziv\Documents\AAA_projects\Calculo de inversion\Calculo-de-la-Rentabilidad\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EBEE169-DBCA-487C-ADB6-9A96B2AB5AE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0343EFA7-69A4-4458-98A1-355BDFE5FCF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="19386" windowHeight="11466" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="19386" windowHeight="11466" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BaseCase" sheetId="8" r:id="rId1"/>
-    <sheet name="Multiplicadores" sheetId="9" r:id="rId2"/>
-    <sheet name="Hoja blanco" sheetId="4" r:id="rId3"/>
+    <sheet name="Hoja blanco" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="31">
   <si>
     <t>Estudio de la rentabilidad: Planta ABC. SA</t>
   </si>
@@ -122,6 +121,12 @@
   </si>
   <si>
     <t>Datos Proyecto multiplicados</t>
+  </si>
+  <si>
+    <t>tipo de multiplicador</t>
+  </si>
+  <si>
+    <t>num_de_multiplicador</t>
   </si>
 </sst>
 </file>
@@ -670,6 +675,17 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{68A68E0C-1B3C-4E97-BFAF-4F4ACCB1EB1D}" name="Table1" displayName="Table1" ref="A32:B35" totalsRowShown="0">
+  <autoFilter ref="A32:B35" xr:uid="{68A68E0C-1B3C-4E97-BFAF-4F4ACCB1EB1D}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{6141B32E-63A2-44F2-83B5-99A5E929F109}" name="tipo de multiplicador"/>
+    <tableColumn id="2" xr3:uid="{93E75B6A-4C4D-40F3-B5D4-B7FA94EEBAD3}" name="num_de_multiplicador"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -959,16 +975,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N29"/>
+  <dimension ref="A1:N35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.52734375" defaultRowHeight="12.7" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="29.41015625" customWidth="1"/>
-    <col min="2" max="2" width="16.87890625" customWidth="1"/>
+    <col min="2" max="2" width="19.17578125" customWidth="1"/>
     <col min="3" max="4" width="12.3515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.87890625" customWidth="1"/>
   </cols>
@@ -1171,31 +1187,31 @@
         <v>70200</v>
       </c>
       <c r="G6" s="19">
-        <f>($B$21*$B$25+$B$22*$B$26)*Multiplicadores!B2</f>
+        <f>($B$21*$B$25+$B$22*$B$26)*BaseCase!B34</f>
         <v>78000</v>
       </c>
       <c r="H6" s="19">
-        <f>($B$21*$B$25+$B$22*$B$26)*Multiplicadores!B2</f>
+        <f>($B$21*$B$25+$B$22*$B$26)*BaseCase!B34</f>
         <v>78000</v>
       </c>
       <c r="I6" s="19">
-        <f>1.05*($B$21*$B$25+$B$22*$B$26)*Multiplicadores!B2</f>
+        <f>1.05*($B$21*$B$25+$B$22*$B$26)*BaseCase!B34</f>
         <v>81900</v>
       </c>
       <c r="J6" s="19">
-        <f>1.05*($B$21*$B$25+$B$22*$B$26)*Multiplicadores!B2</f>
+        <f>1.05*($B$21*$B$25+$B$22*$B$26)*BaseCase!B34</f>
         <v>81900</v>
       </c>
       <c r="K6" s="19">
-        <f>1.05*($B$21*$B$25+$B$22*$B$26)*Multiplicadores!B2</f>
+        <f>1.05*($B$21*$B$25+$B$22*$B$26)*BaseCase!B34</f>
         <v>81900</v>
       </c>
       <c r="L6" s="19">
-        <f>1.05*($B$21*$B$25+$B$22*$B$26)*Multiplicadores!B2</f>
+        <f>1.05*($B$21*$B$25+$B$22*$B$26)*BaseCase!B34</f>
         <v>81900</v>
       </c>
       <c r="M6" s="19">
-        <f t="shared" ref="I6:N6" si="2">1.05*($B$21*$B$25+$B$22*$B$26)</f>
+        <f t="shared" ref="M6:N6" si="2">1.05*($B$21*$B$25+$B$22*$B$26)</f>
         <v>81900</v>
       </c>
       <c r="N6" s="20">
@@ -1217,39 +1233,39 @@
         <v>0</v>
       </c>
       <c r="E7" s="19">
-        <f>SUM(E8:E10)*Multiplicadores!$B$3</f>
+        <f>SUM(E8:E10)*BaseCase!$B$35</f>
         <v>18678.88</v>
       </c>
       <c r="F7" s="19">
-        <f>SUM(F8:F10)*Multiplicadores!$B$3</f>
+        <f>SUM(F8:F10)*BaseCase!$B$35</f>
         <v>22406.655999999999</v>
       </c>
       <c r="G7" s="19">
-        <f>SUM(G8:G10)*Multiplicadores!$B$3</f>
+        <f>SUM(G8:G10)*BaseCase!$B$35</f>
         <v>24891.84</v>
       </c>
       <c r="H7" s="19">
-        <f>SUM(H8:H10)*Multiplicadores!$B$3</f>
+        <f>SUM(H8:H10)*BaseCase!$B$35</f>
         <v>29870.207999999999</v>
       </c>
       <c r="I7" s="19">
-        <f>SUM(I8:I10)*Multiplicadores!$B$3</f>
+        <f>SUM(I8:I10)*BaseCase!$B$35</f>
         <v>29870.207999999999</v>
       </c>
       <c r="J7" s="19">
-        <f>SUM(J8:J10)*Multiplicadores!$B$3</f>
+        <f>SUM(J8:J10)*BaseCase!$B$35</f>
         <v>29870.207999999999</v>
       </c>
       <c r="K7" s="19">
-        <f>SUM(K8:K10)*Multiplicadores!$B$3</f>
+        <f>SUM(K8:K10)*BaseCase!$B$35</f>
         <v>29870.207999999999</v>
       </c>
       <c r="L7" s="19">
-        <f>SUM(L8:L10)*Multiplicadores!$B$3</f>
+        <f>SUM(L8:L10)*BaseCase!$B$35</f>
         <v>29870.207999999999</v>
       </c>
       <c r="M7" s="19">
-        <f t="shared" ref="E7:N7" si="3">SUM(M8:M10)</f>
+        <f t="shared" ref="M7:N7" si="3">SUM(M8:M10)</f>
         <v>29870.207999999999</v>
       </c>
       <c r="N7" s="20">
@@ -1752,7 +1768,7 @@
         <v>140000</v>
       </c>
       <c r="C20" s="1">
-        <f>B20*Multiplicadores!B1</f>
+        <f>B20*BaseCase!B33</f>
         <v>140000</v>
       </c>
       <c r="D20" s="1"/>
@@ -1854,6 +1870,38 @@
       <c r="D29" s="1">
         <f>B29*C29</f>
         <v>4.34</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A32" t="s">
+        <v>29</v>
+      </c>
+      <c r="B32" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A33" t="s">
+        <v>23</v>
+      </c>
+      <c r="B33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A34" t="s">
+        <v>26</v>
+      </c>
+      <c r="B34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A35" t="s">
+        <v>27</v>
+      </c>
+      <c r="B35">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1864,52 +1912,13 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE702265-E10B-4C0E-9313-52523401792C}">
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.7" x14ac:dyDescent="0.4"/>
-  <cols>
-    <col min="1" max="1" width="12.17578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:N29"/>
   <sheetViews>

</xml_diff>